<commit_message>
Update in Summary Excel File
</commit_message>
<xml_diff>
--- a/Americas NLP.xlsx
+++ b/Americas NLP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camtech/Downloads/americasNLP_workshop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85BD3EF-D666-C84F-B036-48D25C4B196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9E4BB0-B771-694C-90EC-7A748853EF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{B5D62453-EC02-934B-B423-9F1D7F75BBA9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{B5D62453-EC02-934B-B423-9F1D7F75BBA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -229,6 +226,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +566,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="183" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="183" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -579,36 +579,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="5"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
@@ -623,60 +623,60 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>5785</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>6</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>23.04</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>8.2899999999999991</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>33.28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>5785</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>7.72</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>24.17</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>8.2899999999999991</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>32.979999999999997</v>
       </c>
     </row>
@@ -710,60 +710,60 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>5672</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>7.28</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>23.06</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>8.2899999999999991</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>32.950000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>5672</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>8.19</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>23.08</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>8.75</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>33.380000000000003</v>
       </c>
     </row>
@@ -797,60 +797,60 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>3862</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>2.65</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>18.18</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>4.0199999999999996</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <v>18.7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>3862</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>2.7</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>18.98</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>2.2200000000000002</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>17.920000000000002</v>
       </c>
     </row>
@@ -882,60 +882,60 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>3805</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>3.02</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>15.99</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>4.78</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>18.21</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>3805</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>3.87</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>15.68</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>3.19</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -969,60 +969,60 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="10">
-        <v>75959</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="9">
+        <v>82218</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <v>11.89</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="10">
         <v>30.94</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>12.5</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="10">
         <v>39.1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="10">
-        <v>75959</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="D16" s="9">
+        <v>82218</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>13.81</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <v>32.619999999999997</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>14.19</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>40.51</v>
       </c>
     </row>
@@ -1054,60 +1054,60 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="10">
-        <v>1376</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="9">
+        <v>7635</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>14.38</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>31.01</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>17.3</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>41.26</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="10">
-        <v>1376</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="D19" s="9">
+        <v>7635</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>15.37</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="10">
         <v>32.06</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <v>18.93</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <v>42.79</v>
       </c>
     </row>
@@ -1141,60 +1141,60 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>75959</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <v>12.36</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <v>31.12</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <v>13.07</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <v>39.18</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="12" t="s">
+      <c r="B22" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <v>75959</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <v>13.43</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="12">
         <v>32.07</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="12">
         <v>13.72</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="12">
         <v>40.43</v>
       </c>
     </row>
@@ -1226,60 +1226,60 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="B24" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <v>1376</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="12">
         <v>41.75</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="12">
         <v>52.67</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="12">
         <v>31.02</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <v>50.76</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="B25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="11">
         <v>1376</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="12">
         <v>42.02</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="12">
         <v>53.83</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="12">
         <v>30.93</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="12">
         <v>49.57</v>
       </c>
     </row>
@@ -1313,60 +1313,60 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="13">
         <v>3260</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="15">
         <v>1.27</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="15">
         <v>20.43</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="15">
         <v>3.08</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27" s="15">
         <v>27.21</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="13">
         <v>3260</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <v>0.78</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="15">
         <v>21.15</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="15">
         <v>1.08</v>
       </c>
-      <c r="I28" s="16">
+      <c r="I28" s="15">
         <v>27.38</v>
       </c>
     </row>
@@ -1398,60 +1398,60 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>212</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="15">
         <v>0.74</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="15">
         <v>19.21</v>
       </c>
-      <c r="H30" s="16">
+      <c r="H30" s="15">
         <v>1.86</v>
       </c>
-      <c r="I30" s="16">
+      <c r="I30" s="15">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="13">
         <v>212</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="15">
         <v>1.71</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G31" s="15">
         <v>18.399999999999999</v>
       </c>
-      <c r="H31" s="16">
+      <c r="H31" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I31" s="16">
+      <c r="I31" s="15">
         <v>29.3</v>
       </c>
     </row>

</xml_diff>